<commit_message>
messing with catch data, but final processing ended up in R data prep script
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Adjusted_Nisqually_Chinook_and_Chum_from_Craig_July2024 and August.xlsx
+++ b/Data/Nisqually/Adjusted_Nisqually_Chinook_and_Chum_from_Craig_July2024 and August.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B724F40-6AD3-4F4D-930B-68E0FBD94CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7158F19F-D2BA-4E18-80AA-A564EBB8F224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28410" yWindow="5625" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="1" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
+    <workbookView xWindow="-28410" yWindow="5625" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="3" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="GR Chinook" sheetId="2" r:id="rId2"/>
     <sheet name="LocNis Chinook" sheetId="3" r:id="rId3"/>
     <sheet name="Winter Chum" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5486,8 +5487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5AB5EB-5F17-4CB3-ADB0-B51E1B4ACDBA}">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:U21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7214,8 +7215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A7BE78-C8A2-4AA0-A137-4EE20A67C024}">
   <dimension ref="A1:Y70"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7225,13 +7226,13 @@
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7367,8 +7368,8 @@
         <v>30.570340662095699</v>
       </c>
       <c r="I6" s="27">
-        <f t="shared" ref="I6:I15" si="1">H6/E6</f>
-        <v>5.8988088016300559E-2</v>
+        <f>X6</f>
+        <v>7.1671356952847307E-2</v>
       </c>
       <c r="J6">
         <f>H6/E6</f>
@@ -7427,12 +7428,12 @@
         <v>304.25361536533006</v>
       </c>
       <c r="X6">
-        <f>AVERAGE(V6,T6,R6,P6,N6,L6,J6)</f>
-        <v>7.3199255981372016E-2</v>
+        <f>H6/AVERAGE(E6,K6,M6,O6,Q6,S6,U6)</f>
+        <v>7.1671356952847307E-2</v>
       </c>
       <c r="Y6">
-        <f>X6*E6</f>
-        <v>37.935221615322121</v>
+        <f>X6*AVERAGE(U6,E6)</f>
+        <v>30.570340662095692</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -7447,14 +7448,14 @@
         <v>0.04</v>
       </c>
       <c r="E7" s="41">
-        <f t="shared" ref="E7:E15" si="2">D7*E$3</f>
+        <f t="shared" ref="E7:E15" si="1">D7*E$3</f>
         <v>1036.492</v>
       </c>
       <c r="F7" s="67">
         <v>3.0043293288352257E-2</v>
       </c>
       <c r="G7" s="58">
-        <f t="shared" ref="G7:G14" si="3">F7*E$3</f>
+        <f t="shared" ref="G7:G14" si="2">F7*E$3</f>
         <v>778.49082867577022</v>
       </c>
       <c r="H7">
@@ -7462,8 +7463,68 @@
         <v>111.21297552511002</v>
       </c>
       <c r="I7" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I7:I15" si="3">X7</f>
+        <v>0.15823075935802897</v>
+      </c>
+      <c r="J7">
+        <f>H7/E7</f>
         <v>0.10729747602982949</v>
+      </c>
+      <c r="K7" s="13">
+        <f>E7-H7</f>
+        <v>925.27902447488998</v>
+      </c>
+      <c r="L7">
+        <f>H7/K7</f>
+        <v>0.12019398752524958</v>
+      </c>
+      <c r="M7" s="13">
+        <f>K7-H7</f>
+        <v>814.06604894978</v>
+      </c>
+      <c r="N7">
+        <f>H7/M7</f>
+        <v>0.13661419201621905</v>
+      </c>
+      <c r="O7" s="13">
+        <f>M7-H7</f>
+        <v>702.85307342467001</v>
+      </c>
+      <c r="P7">
+        <f>H7/O7</f>
+        <v>0.15823075935802897</v>
+      </c>
+      <c r="Q7" s="13">
+        <f>O7-H7</f>
+        <v>591.64009789956003</v>
+      </c>
+      <c r="R7">
+        <f>H7/Q7</f>
+        <v>0.18797403340297286</v>
+      </c>
+      <c r="S7" s="13">
+        <f>Q7-H7</f>
+        <v>480.42712237444999</v>
+      </c>
+      <c r="T7">
+        <f>H7/S7</f>
+        <v>0.23148771238279395</v>
+      </c>
+      <c r="U7" s="13">
+        <f>S7-H7</f>
+        <v>369.21414684933995</v>
+      </c>
+      <c r="V7">
+        <f>H7/U7</f>
+        <v>0.30121536911339192</v>
+      </c>
+      <c r="W7" s="13">
+        <f>U7-H7</f>
+        <v>258.00117132422992</v>
+      </c>
+      <c r="X7">
+        <f>H7/AVERAGE(E7,K7,M7,O7,Q7,S7,U7)</f>
+        <v>0.15823075935802897</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -7478,23 +7539,83 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2591.23</v>
       </c>
       <c r="F8" s="67">
         <v>2.9188024261888126E-2</v>
       </c>
       <c r="G8" s="58">
+        <f t="shared" si="2"/>
+        <v>756.32884108132362</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>108.04697729733195</v>
+      </c>
+      <c r="I8" s="27">
         <f t="shared" si="3"/>
-        <v>756.32884108132362</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>108.04697729733195</v>
-      </c>
-      <c r="I8" s="27">
-        <f t="shared" si="1"/>
+        <v>4.7658902694768142E-2</v>
+      </c>
+      <c r="J8">
+        <f>H8/E8</f>
         <v>4.1697177516983035E-2</v>
+      </c>
+      <c r="K8" s="13">
+        <f>E8-H8</f>
+        <v>2483.183022702668</v>
+      </c>
+      <c r="L8">
+        <f>H8/K8</f>
+        <v>4.3511483571490775E-2</v>
+      </c>
+      <c r="M8" s="13">
+        <f>K8-H8</f>
+        <v>2375.1360454053361</v>
+      </c>
+      <c r="N8">
+        <f>H8/M8</f>
+        <v>4.5490858305294618E-2</v>
+      </c>
+      <c r="O8" s="13">
+        <f>M8-H8</f>
+        <v>2267.0890681080041</v>
+      </c>
+      <c r="P8">
+        <f>H8/O8</f>
+        <v>4.7658902694768142E-2</v>
+      </c>
+      <c r="Q8" s="13">
+        <f>O8-H8</f>
+        <v>2159.0420908106721</v>
+      </c>
+      <c r="R8">
+        <f>H8/Q8</f>
+        <v>5.0043942059861707E-2</v>
+      </c>
+      <c r="S8" s="13">
+        <f>Q8-H8</f>
+        <v>2050.9951135133401</v>
+      </c>
+      <c r="T8">
+        <f>H8/S8</f>
+        <v>5.2680270462589371E-2</v>
+      </c>
+      <c r="U8" s="13">
+        <f>S8-H8</f>
+        <v>1942.9481362160082</v>
+      </c>
+      <c r="V8">
+        <f>H8/U8</f>
+        <v>5.5609810310098665E-2</v>
+      </c>
+      <c r="W8" s="13">
+        <f>U8-H8</f>
+        <v>1834.9011589186762</v>
+      </c>
+      <c r="X8">
+        <f>H8/AVERAGE(E8,K8,M8,O8,Q8,S8,U8)</f>
+        <v>4.7658902694768142E-2</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -7509,23 +7630,83 @@
         <v>0.17</v>
       </c>
       <c r="E9" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4405.0910000000003</v>
       </c>
       <c r="F9" s="67">
         <v>4.0593812603886177E-2</v>
       </c>
       <c r="G9" s="58">
+        <f t="shared" si="2"/>
+        <v>1051.8790503356797</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>150.26843576223996</v>
+      </c>
+      <c r="I9" s="27">
         <f t="shared" si="3"/>
-        <v>1051.8790503356797</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>150.26843576223996</v>
-      </c>
-      <c r="I9" s="27">
-        <f t="shared" si="1"/>
+        <v>3.8001410985338158E-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9:J15" si="4">H9/E9</f>
         <v>3.41124475662909E-2</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" ref="K9:K15" si="5">E9-H9</f>
+        <v>4254.8225642377602</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L15" si="6">H9/K9</f>
+        <v>3.5317203830134369E-2</v>
+      </c>
+      <c r="M9" s="13">
+        <f t="shared" ref="M9:M15" si="7">K9-H9</f>
+        <v>4104.55412847552</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9:N15" si="8">H9/M9</f>
+        <v>3.6610172763893223E-2</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" ref="O9:O15" si="9">M9-H9</f>
+        <v>3954.2856927132798</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P15" si="10">H9/O9</f>
+        <v>3.8001410985338165E-2</v>
+      </c>
+      <c r="Q9" s="13">
+        <f t="shared" ref="Q9:Q15" si="11">O9-H9</f>
+        <v>3804.0172569510396</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ref="R9:R15" si="12">H9/Q9</f>
+        <v>3.9502564160994819E-2</v>
+      </c>
+      <c r="S9" s="13">
+        <f t="shared" ref="S9:S15" si="13">Q9-H9</f>
+        <v>3653.7488211887994</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ref="T9:T15" si="14">H9/S9</f>
+        <v>4.1127193771724017E-2</v>
+      </c>
+      <c r="U9" s="13">
+        <f t="shared" ref="U9:U15" si="15">S9-H9</f>
+        <v>3503.4803854265592</v>
+      </c>
+      <c r="V9">
+        <f t="shared" ref="V9:V15" si="16">H9/U9</f>
+        <v>4.289118797048562E-2</v>
+      </c>
+      <c r="W9" s="13">
+        <f t="shared" ref="W9:W15" si="17">U9-H9</f>
+        <v>3353.211949664319</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ref="X9:X15" si="18">H9/AVERAGE(E9,K9,M9,O9,Q9,S9,U9)</f>
+        <v>3.8001410985338158E-2</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -7540,23 +7721,83 @@
         <v>0.21</v>
       </c>
       <c r="E10" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5441.5829999999996</v>
       </c>
       <c r="F10" s="67">
         <v>4.5248433163820295E-2</v>
       </c>
       <c r="G10" s="58">
+        <f t="shared" si="2"/>
+        <v>1172.4909746708606</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>167.49871066726581</v>
+      </c>
+      <c r="I10" s="27">
         <f t="shared" si="3"/>
-        <v>1172.4909746708606</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>167.49871066726581</v>
-      </c>
-      <c r="I10" s="27">
-        <f t="shared" si="1"/>
+        <v>3.3912890204976814E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
         <v>3.078124705021789E-2</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" si="5"/>
+        <v>5274.0842893327335</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="6"/>
+        <v>3.1758823234214445E-2</v>
+      </c>
+      <c r="M10" s="13">
+        <f t="shared" si="7"/>
+        <v>5106.5855786654674</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="8"/>
+        <v>3.2800529451038632E-2</v>
+      </c>
+      <c r="O10" s="13">
+        <f t="shared" si="9"/>
+        <v>4939.0868679982013</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="10"/>
+        <v>3.3912890204976814E-2</v>
+      </c>
+      <c r="Q10" s="13">
+        <f t="shared" si="11"/>
+        <v>4771.5881573309352</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="12"/>
+        <v>3.5103346128044485E-2</v>
+      </c>
+      <c r="S10" s="13">
+        <f t="shared" si="13"/>
+        <v>4604.0894466636692</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="14"/>
+        <v>3.638042062554691E-2</v>
+      </c>
+      <c r="U10" s="13">
+        <f t="shared" si="15"/>
+        <v>4436.5907359964031</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="16"/>
+        <v>3.7753924270783043E-2</v>
+      </c>
+      <c r="W10" s="13">
+        <f t="shared" si="17"/>
+        <v>4269.092025329137</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="18"/>
+        <v>3.3912890204976814E-2</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -7571,23 +7812,83 @@
         <v>0.19</v>
       </c>
       <c r="E11" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4923.3369999999995</v>
       </c>
       <c r="F11" s="67">
         <v>4.0808034301407836E-2</v>
       </c>
       <c r="G11" s="58">
+        <f t="shared" si="2"/>
+        <v>1057.4300272283701</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>151.06143246119572</v>
+      </c>
+      <c r="I11" s="27">
         <f t="shared" si="3"/>
-        <v>1057.4300272283701</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>151.06143246119572</v>
-      </c>
-      <c r="I11" s="27">
-        <f t="shared" si="1"/>
+        <v>3.3793349469421578E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
         <v>3.0682732557449497E-2</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" si="5"/>
+        <v>4772.2755675388034</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="6"/>
+        <v>3.1653962627120953E-2</v>
+      </c>
+      <c r="M11" s="13">
+        <f t="shared" si="7"/>
+        <v>4621.2141350776074</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="8"/>
+        <v>3.2688689172517396E-2</v>
+      </c>
+      <c r="O11" s="13">
+        <f t="shared" si="9"/>
+        <v>4470.1527026164113</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="10"/>
+        <v>3.3793349469421578E-2</v>
+      </c>
+      <c r="Q11" s="13">
+        <f t="shared" si="11"/>
+        <v>4319.0912701552152</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="12"/>
+        <v>3.4975281375743426E-2</v>
+      </c>
+      <c r="S11" s="13">
+        <f t="shared" si="13"/>
+        <v>4168.0298376940191</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="14"/>
+        <v>3.6242886529999296E-2</v>
+      </c>
+      <c r="U11" s="13">
+        <f t="shared" si="15"/>
+        <v>4016.9684052328234</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="16"/>
+        <v>3.7605830373077132E-2</v>
+      </c>
+      <c r="W11" s="13">
+        <f t="shared" si="17"/>
+        <v>3865.9069727716278</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="18"/>
+        <v>3.3793349469421578E-2</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -7602,23 +7903,83 @@
         <v>0.15</v>
       </c>
       <c r="E12" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3886.8449999999998</v>
       </c>
       <c r="F12" s="67">
         <v>9.6831624641389481E-3</v>
       </c>
       <c r="G12" s="58">
+        <f t="shared" si="2"/>
+        <v>250.91301071950767</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>35.844715817072526</v>
+      </c>
+      <c r="I12" s="27">
         <f t="shared" si="3"/>
-        <v>250.91301071950767</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>35.844715817072526</v>
-      </c>
-      <c r="I12" s="27">
-        <f t="shared" si="1"/>
+        <v>9.4844582029812927E-3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
         <v>9.2220594896561415E-3</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" si="5"/>
+        <v>3851.0002841829273</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="6"/>
+        <v>9.307897473883919E-3</v>
+      </c>
+      <c r="M12" s="13">
+        <f t="shared" si="7"/>
+        <v>3815.1555683658548</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="8"/>
+        <v>9.3953484136495881E-3</v>
+      </c>
+      <c r="O12" s="13">
+        <f t="shared" si="9"/>
+        <v>3779.3108525487823</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="10"/>
+        <v>9.4844582029812944E-3</v>
+      </c>
+      <c r="Q12" s="13">
+        <f t="shared" si="11"/>
+        <v>3743.4661367317099</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="12"/>
+        <v>9.5752744936988526E-3</v>
+      </c>
+      <c r="S12" s="13">
+        <f t="shared" si="13"/>
+        <v>3707.6214209146374</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="14"/>
+        <v>9.6678467803840533E-3</v>
+      </c>
+      <c r="U12" s="13">
+        <f t="shared" si="15"/>
+        <v>3671.7767050975649</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="16"/>
+        <v>9.7622264903279507E-3</v>
+      </c>
+      <c r="W12" s="13">
+        <f t="shared" si="17"/>
+        <v>3635.9319892804924</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="18"/>
+        <v>9.4844582029812927E-3</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -7633,23 +7994,83 @@
         <v>0.09</v>
       </c>
       <c r="E13" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2332.107</v>
       </c>
       <c r="F13" s="67">
         <v>4.4574321975344028E-2</v>
       </c>
       <c r="G13" s="58">
+        <f t="shared" si="2"/>
+        <v>1155.0232033217071</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>165.00331476024388</v>
+      </c>
+      <c r="I13" s="27">
         <f t="shared" si="3"/>
-        <v>1155.0232033217071</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>165.00331476024388</v>
-      </c>
-      <c r="I13" s="27">
-        <f t="shared" si="1"/>
+        <v>8.9817418326676862E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
         <v>7.0752892024355613E-2</v>
+      </c>
+      <c r="K13" s="13">
+        <f t="shared" si="5"/>
+        <v>2167.103685239756</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>7.6140018534456441E-2</v>
+      </c>
+      <c r="M13" s="13">
+        <f t="shared" si="7"/>
+        <v>2002.1003704795121</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="8"/>
+        <v>8.2415106252003156E-2</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" si="9"/>
+        <v>1837.0970557192682</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="10"/>
+        <v>8.9817418326676848E-2</v>
+      </c>
+      <c r="Q13" s="13">
+        <f t="shared" si="11"/>
+        <v>1672.0937409590242</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="12"/>
+        <v>9.8680660490725089E-2</v>
+      </c>
+      <c r="S13" s="13">
+        <f t="shared" si="13"/>
+        <v>1507.0904261987803</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="14"/>
+        <v>0.10948468113915315</v>
+      </c>
+      <c r="U13" s="13">
+        <f t="shared" si="15"/>
+        <v>1342.0871114385363</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="16"/>
+        <v>0.12294530910395421</v>
+      </c>
+      <c r="W13" s="13">
+        <f t="shared" si="17"/>
+        <v>1177.0837966782924</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="18"/>
+        <v>8.9817418326676862E-2</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -7664,23 +8085,83 @@
         <v>0.02</v>
       </c>
       <c r="E14" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>518.24599999999998</v>
       </c>
       <c r="F14" s="67">
         <v>1.0152827255278366E-2</v>
       </c>
       <c r="G14" s="58">
+        <f t="shared" si="2"/>
+        <v>263.08310568694958</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>37.583300812421371</v>
+      </c>
+      <c r="I14" s="27">
         <f t="shared" si="3"/>
-        <v>263.08310568694958</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>37.583300812421371</v>
-      </c>
-      <c r="I14" s="27">
-        <f t="shared" si="1"/>
+        <v>9.2684741082142502E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
         <v>7.2520194680559757E-2</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" si="5"/>
+        <v>480.6626991875786</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
+        <v>7.8190591606016199E-2</v>
+      </c>
+      <c r="M14" s="13">
+        <f t="shared" si="7"/>
+        <v>443.07939837515721</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="8"/>
+        <v>8.4822948099697995E-2</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="9"/>
+        <v>405.49609756273583</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="10"/>
+        <v>9.2684741082142516E-2</v>
+      </c>
+      <c r="Q14" s="13">
+        <f t="shared" si="11"/>
+        <v>367.91279675031444</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="12"/>
+        <v>0.10215274147674573</v>
+      </c>
+      <c r="S14" s="13">
+        <f t="shared" si="13"/>
+        <v>330.32949593789306</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="14"/>
+        <v>0.11377518893888786</v>
+      </c>
+      <c r="U14" s="13">
+        <f t="shared" si="15"/>
+        <v>292.74619512547167</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="16"/>
+        <v>0.12838185922899215</v>
+      </c>
+      <c r="W14" s="13">
+        <f t="shared" si="17"/>
+        <v>255.16289431305029</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="18"/>
+        <v>9.2684741082142502E-2</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -7695,7 +8176,7 @@
         <v>0.01</v>
       </c>
       <c r="E15" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>259.12299999999999</v>
       </c>
       <c r="F15" s="40"/>
@@ -7705,7 +8186,67 @@
         <v>0</v>
       </c>
       <c r="I15" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" si="5"/>
+        <v>259.12299999999999</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="13">
+        <f t="shared" si="7"/>
+        <v>259.12299999999999</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="9"/>
+        <v>259.12299999999999</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="13">
+        <f t="shared" si="11"/>
+        <v>259.12299999999999</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="13">
+        <f t="shared" si="13"/>
+        <v>259.12299999999999</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="13">
+        <f t="shared" si="15"/>
+        <v>259.12299999999999</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="13">
+        <f t="shared" si="17"/>
+        <v>259.12299999999999</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -7883,14 +8424,14 @@
         <v>4.1877009175387586E-2</v>
       </c>
       <c r="E32" s="35">
-        <f t="shared" ref="E32:E41" si="4">D32*E$29</f>
+        <f t="shared" ref="E32:E41" si="19">D32*E$29</f>
         <v>2634.8930419135518</v>
       </c>
       <c r="F32" s="40">
         <v>1.7322391525776124E-2</v>
       </c>
       <c r="G32" s="61">
-        <f t="shared" ref="G32:G41" si="5">E$29*F32</f>
+        <f t="shared" ref="G32:G41" si="20">E$29*F32</f>
         <v>1089.9214103235286</v>
       </c>
       <c r="H32" s="35"/>
@@ -7908,14 +8449,14 @@
         <v>0.13755231785047886</v>
       </c>
       <c r="E33" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>8654.7643286885595</v>
       </c>
       <c r="F33" s="40">
         <v>5.4890886049515149E-2</v>
       </c>
       <c r="G33" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>3453.7235720582835</v>
       </c>
       <c r="H33" s="35"/>
@@ -7933,14 +8474,14 @@
         <v>0.19396780095362728</v>
       </c>
       <c r="E34" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>12204.415242442039</v>
       </c>
       <c r="F34" s="40">
         <v>7.8647474562515154E-2</v>
       </c>
       <c r="G34" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>4948.4833699785413</v>
       </c>
       <c r="H34" s="35"/>
@@ -7958,14 +8499,14 @@
         <v>0.20311899983834181</v>
       </c>
       <c r="E35" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>12780.206846028499</v>
       </c>
       <c r="F35" s="40">
         <v>8.440563621052824E-2</v>
       </c>
       <c r="G35" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>5310.785749239195</v>
       </c>
       <c r="H35" s="35"/>
@@ -7983,14 +8524,14 @@
         <v>0.17847712529832935</v>
       </c>
       <c r="E36" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>11229.745028345824</v>
       </c>
       <c r="F36" s="40">
         <v>7.7517292720955977E-2</v>
       </c>
       <c r="G36" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>4877.3725545440066</v>
       </c>
       <c r="H36" s="35"/>
@@ -8008,14 +8549,14 @@
         <v>0.12613381037007415</v>
       </c>
       <c r="E37" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>7936.3141217229922</v>
       </c>
       <c r="F37" s="40">
         <v>7.3840269091484848E-2</v>
       </c>
       <c r="G37" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>4646.0149631824088</v>
       </c>
       <c r="H37" s="35"/>
@@ -8033,14 +8574,14 @@
         <v>7.5793773952497437E-2</v>
       </c>
       <c r="E38" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>4768.929098336348</v>
       </c>
       <c r="F38" s="40">
         <v>4.926434994082958E-2</v>
       </c>
       <c r="G38" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>3099.7030454070091</v>
       </c>
       <c r="H38" s="35"/>
@@ -8058,14 +8599,14 @@
         <v>1.7041651638824873E-2</v>
       </c>
       <c r="E39" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>1072.2573127845333</v>
       </c>
       <c r="F39" s="40">
         <v>1.5211570171496427E-2</v>
       </c>
       <c r="G39" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>957.1089528765209</v>
       </c>
       <c r="H39" s="35"/>
@@ -8083,14 +8624,14 @@
         <v>1.0209184029856589E-2</v>
       </c>
       <c r="E40" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>642.35981732177061</v>
       </c>
       <c r="F40" s="40">
         <v>1.3452779023284905E-2</v>
       </c>
       <c r="G40" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>846.44616558928158</v>
       </c>
       <c r="H40" s="35"/>
@@ -8108,14 +8649,14 @@
         <v>6.9823824147405853E-4</v>
       </c>
       <c r="E41" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>43.933010505899468</v>
       </c>
       <c r="F41" s="40">
         <v>2.5121756196845244E-3</v>
       </c>
       <c r="G41" s="61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>158.06558755542633</v>
       </c>
       <c r="H41" s="40"/>
@@ -8276,6 +8817,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C215CA6E-CE6F-4229-AF8E-ABAE683A4B5C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
small data messing around
</commit_message>
<xml_diff>
--- a/Data/Nisqually/Adjusted_Nisqually_Chinook_and_Chum_from_Craig_July2024 and August.xlsx
+++ b/Data/Nisqually/Adjusted_Nisqually_Chinook_and_Chum_from_Craig_July2024 and August.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Nisqually\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7158F19F-D2BA-4E18-80AA-A564EBB8F224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9F15E9-9957-4531-977C-FDB37D517CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28410" yWindow="5625" windowWidth="24720" windowHeight="14355" firstSheet="1" activeTab="3" xr2:uid="{92F3D677-A32A-4EE8-AC44-3E7A0B434AE3}"/>
   </bookViews>
@@ -5458,17 +5458,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
@@ -5477,6 +5466,17 @@
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A62:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8833,20 +8833,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f5b128de-c6a3-4183-b93b-b89b90348e84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9050,6 +9050,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963F9B2A-3B8E-4C64-9F16-4BF0FA3AF67D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9061,14 +9069,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63CBB38-F76E-4FFA-88CB-BC1901B39799}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>